<commit_message>
Atualização Atividade 2 - Lista de Variaveis
Listagem da Classe ServicoPrestadoTeste.java.
</commit_message>
<xml_diff>
--- a/Atividade 2 - Lista de variáveis _ Italo.xlsx
+++ b/Atividade 2 - Lista de variáveis _ Italo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="15150" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="15150" windowHeight="7995" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="View" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="288">
   <si>
     <t>Class</t>
   </si>
@@ -912,6 +912,447 @@
   </si>
   <si>
     <t>JLabel object that refers to the icon of 'Barbearia Peixoto' logo.</t>
+  </si>
+  <si>
+    <t>ServicoPrestadoTeste.java</t>
+  </si>
+  <si>
+    <t>DoneServiceTest.java</t>
+  </si>
+  <si>
+    <t>Instance of 'ServicoPrestado' class</t>
+  </si>
+  <si>
+    <t>testeDeConstrutor</t>
+  </si>
+  <si>
+    <t>constructorTest</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test the class constructor</t>
+    </r>
+  </si>
+  <si>
+    <t>servico1</t>
+  </si>
+  <si>
+    <t>service1</t>
+  </si>
+  <si>
+    <t>Instance of 'ServicoPrestado' class used to test the constructor</t>
+  </si>
+  <si>
+    <t>testeSetNomeNaoNulo</t>
+  </si>
+  <si>
+    <t>testeSetNomeBranco</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'nomeServico' don't accept blank names</t>
+    </r>
+  </si>
+  <si>
+    <t>testeSetNomeForaDeFormato</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'nomeServico' don't accept nonstandard names</t>
+    </r>
+  </si>
+  <si>
+    <t>testeSetNomeValido</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'nomeServico' accept legal names and test the setter result</t>
+    </r>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>serviceException</t>
+  </si>
+  <si>
+    <t>Variable that stores a possible exception from 'ServicoException.java' type</t>
+  </si>
+  <si>
+    <t>precoForaDeFormato</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'preco' accept legal prices and test the setter result</t>
+    </r>
+  </si>
+  <si>
+    <t>setterDoneServicePriceTestForInvalidArgument</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'preco' don't accept ilegal prices</t>
+    </r>
+  </si>
+  <si>
+    <t>testePrecoNaoNulo</t>
+  </si>
+  <si>
+    <t>setterDoneServiceNomeTestValidArgument</t>
+  </si>
+  <si>
+    <t>setterDoneServiceNameTestForInvalidArgument</t>
+  </si>
+  <si>
+    <t>setterDoneServiceNameTestForBlankArgument</t>
+  </si>
+  <si>
+    <t>setterDoneServiceNameTestForNullArgument</t>
+  </si>
+  <si>
+    <t>setterDoneServicePriceTestForNullArgument</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'preco' don't accept null argument</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'nomeServico' don't accept null argument</t>
+    </r>
+  </si>
+  <si>
+    <t>testePrecoEmBranco</t>
+  </si>
+  <si>
+    <t>setterDoneServicePriceTestForBlankArgument</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'preco' don't accept blank prices</t>
+    </r>
+  </si>
+  <si>
+    <t>testePrecoValido</t>
+  </si>
+  <si>
+    <t>setterDoneServicePriceTestForValidArgument</t>
+  </si>
+  <si>
+    <t>testeNomeBarbeiroNulo</t>
+  </si>
+  <si>
+    <t>setterBarberNameTestForNullArgument</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'nomeBarbeiro' don't accept null argument</t>
+    </r>
+  </si>
+  <si>
+    <t>testeNomeBarbeiroEmBranco</t>
+  </si>
+  <si>
+    <t>setterBarberNameTestForBlankArgument</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'nomeBarbeiro' don't accept blank barber names</t>
+    </r>
+  </si>
+  <si>
+    <t>testeNomeBarbeiroForaDeFormato</t>
+  </si>
+  <si>
+    <t>setterBarberNameTestForInvalidArgument</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'nomeBarbeiro' don't accept ilegal names</t>
+    </r>
+  </si>
+  <si>
+    <t>testeNomeBarbeiroValido</t>
+  </si>
+  <si>
+    <t>setterBarberNameTestForValidArgument</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'nomeBarbeiro' accept legal names and test the setter result</t>
+    </r>
+  </si>
+  <si>
+    <t>testeDataNulo</t>
+  </si>
+  <si>
+    <t>setterDoneServiceDateTestForNullArgument</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'data' don't accept null arguments</t>
+    </r>
+  </si>
+  <si>
+    <t>parseException</t>
+  </si>
+  <si>
+    <t>assertFailedException</t>
+  </si>
+  <si>
+    <t>Variable that stores a possible exception from 'ParseException' type</t>
+  </si>
+  <si>
+    <t>Variable that stores a possible exception from 'AssertionFailedError' type</t>
+  </si>
+  <si>
+    <t>testeDataEmBranco</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>setterDoneServiceDateTestForBlankArgument</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'data' don't accept blank date</t>
+    </r>
+  </si>
+  <si>
+    <t>testeDataForaDeFormato</t>
+  </si>
+  <si>
+    <t>setterDoneServiceDateTestForInvalidArgument</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'data' don't accept ilegal types of date</t>
+    </r>
+  </si>
+  <si>
+    <t>testeDataParaConverter</t>
+  </si>
+  <si>
+    <t>dateConversionToAbntTest</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the date conversion to ABNT format is correct. Stores Parse Exception</t>
+    </r>
+  </si>
+  <si>
+    <t>testeDataNormal</t>
+  </si>
+  <si>
+    <t>setterDoneServiceDateTestForValidArgument</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the setter of 'data' accept legal types of date</t>
+    </r>
+  </si>
+  <si>
+    <t>getterDeDataDeveFuncionar</t>
+  </si>
+  <si>
+    <t>getterDoneServiceDateTest</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method name-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test if the getter of 'data' returns the true inserted date</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -983,7 +1424,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -1319,11 +1760,100 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1352,15 +1882,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1371,6 +1892,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1391,16 +1936,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1418,25 +1969,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1735,7 +2292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -1773,10 +2330,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="22" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -1796,8 +2353,8 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="21"/>
-      <c r="B3" s="18"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="8" t="s">
         <v>196</v>
       </c>
@@ -1815,29 +2372,29 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="21"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="36" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="D4" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="13" t="s">
+      <c r="D4" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="21"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="6" t="s">
         <v>201</v>
       </c>
@@ -1849,10 +2406,10 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="21"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
       <c r="E6" s="6" t="s">
         <v>204</v>
       </c>
@@ -1864,10 +2421,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="21"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="6" t="s">
         <v>206</v>
       </c>
@@ -1879,10 +2436,10 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="21"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="6" t="s">
         <v>197</v>
       </c>
@@ -1894,10 +2451,10 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="21"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
       <c r="E9" s="6" t="s">
         <v>210</v>
       </c>
@@ -1909,10 +2466,10 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="22"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="6" t="s">
         <v>214</v>
       </c>
@@ -1924,13 +2481,13 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="4"/>
@@ -2362,8 +2919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B37"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2399,16 +2956,16 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="35" t="s">
+      <c r="C2" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="33" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -2422,10 +2979,10 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="21"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="6" t="s">
         <v>90</v>
       </c>
@@ -2437,10 +2994,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="21"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="6" t="s">
         <v>91</v>
       </c>
@@ -2452,10 +3009,10 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="21"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="6" t="s">
         <v>15</v>
       </c>
@@ -2467,10 +3024,10 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="21"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="6" t="s">
         <v>92</v>
       </c>
@@ -2482,10 +3039,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="21"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="6" t="s">
         <v>93</v>
       </c>
@@ -2497,10 +3054,10 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="21"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="6" t="s">
         <v>94</v>
       </c>
@@ -2512,10 +3069,10 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="21"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="6" t="s">
         <v>95</v>
       </c>
@@ -2527,29 +3084,29 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="21"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="36" t="s">
+      <c r="A10" s="26"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="13" t="s">
+      <c r="E10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="21"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="6" t="s">
         <v>89</v>
       </c>
@@ -2561,10 +3118,10 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="21"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="6" t="s">
         <v>90</v>
       </c>
@@ -2576,10 +3133,10 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="21"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="6" t="s">
         <v>91</v>
       </c>
@@ -2591,10 +3148,10 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="21"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
       <c r="E14" s="6" t="s">
         <v>15</v>
       </c>
@@ -2606,27 +3163,27 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="21"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="14" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="13" t="s">
+      <c r="E15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="21"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="8" t="s">
         <v>111</v>
       </c>
@@ -2644,12 +3201,12 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="21"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="10" t="s">
+      <c r="A17" s="26"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="28" t="s">
         <v>115</v>
       </c>
       <c r="E17" s="6" t="s">
@@ -2663,10 +3220,10 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="21"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
       <c r="E18" s="6" t="s">
         <v>117</v>
       </c>
@@ -2678,10 +3235,10 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="21"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
       <c r="E19" s="6" t="s">
         <v>119</v>
       </c>
@@ -2693,10 +3250,10 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="21"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="6" t="s">
         <v>122</v>
       </c>
@@ -2708,10 +3265,10 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="21"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="6" t="s">
         <v>124</v>
       </c>
@@ -2723,8 +3280,8 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="21"/>
-      <c r="B22" s="18"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="8" t="s">
         <v>127</v>
       </c>
@@ -2742,12 +3299,12 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="21"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="10" t="s">
+      <c r="A23" s="26"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="28" t="s">
         <v>131</v>
       </c>
       <c r="E23" s="6" t="s">
@@ -2761,10 +3318,10 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="21"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="6" t="s">
         <v>117</v>
       </c>
@@ -2776,10 +3333,10 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="21"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="6" t="s">
         <v>119</v>
       </c>
@@ -2791,10 +3348,10 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="21"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
       <c r="E26" s="6" t="s">
         <v>122</v>
       </c>
@@ -2806,10 +3363,10 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="21"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="6" t="s">
         <v>124</v>
       </c>
@@ -2821,8 +3378,8 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="21"/>
-      <c r="B28" s="18"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="8" t="s">
         <v>136</v>
       </c>
@@ -2840,8 +3397,8 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="21"/>
-      <c r="B29" s="18"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="8" t="s">
         <v>137</v>
       </c>
@@ -2859,8 +3416,8 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="21"/>
-      <c r="B30" s="18"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="8" t="s">
         <v>142</v>
       </c>
@@ -2878,8 +3435,8 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="21"/>
-      <c r="B31" s="18"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="23"/>
       <c r="C31" s="8" t="s">
         <v>143</v>
       </c>
@@ -2897,12 +3454,12 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="21"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="10" t="s">
+      <c r="A32" s="26"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="28" t="s">
         <v>149</v>
       </c>
       <c r="E32" s="6" t="s">
@@ -2916,10 +3473,10 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="21"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
       <c r="E33" s="6" t="s">
         <v>151</v>
       </c>
@@ -2931,10 +3488,10 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="21"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
       <c r="E34" s="6" t="s">
         <v>117</v>
       </c>
@@ -2946,10 +3503,10 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="21"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
       <c r="E35" s="6" t="s">
         <v>124</v>
       </c>
@@ -2961,10 +3518,10 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="21"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
       <c r="E36" s="6" t="s">
         <v>122</v>
       </c>
@@ -2976,10 +3533,10 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="22"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="6" t="s">
         <v>154</v>
       </c>
@@ -2991,25 +3548,25 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="23"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="34" t="s">
+      <c r="A39" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="B39" s="33" t="s">
+      <c r="B39" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="C39" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="10" t="s">
+      <c r="C39" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E39" s="6" t="s">
@@ -3023,10 +3580,10 @@
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="21"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
       <c r="E40" s="6" t="s">
         <v>161</v>
       </c>
@@ -3038,10 +3595,10 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="21"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
       <c r="E41" s="6" t="s">
         <v>162</v>
       </c>
@@ -3053,10 +3610,10 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="21"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
       <c r="E42" s="6" t="s">
         <v>163</v>
       </c>
@@ -3068,10 +3625,10 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="21"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
       <c r="E43" s="6" t="s">
         <v>164</v>
       </c>
@@ -3083,10 +3640,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="21"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
       <c r="E44" s="6" t="s">
         <v>165</v>
       </c>
@@ -3098,27 +3655,27 @@
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="21"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="14" t="s">
+      <c r="A45" s="26"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="D45" s="14" t="s">
+      <c r="D45" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="E45" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F45" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G45" s="13" t="s">
+      <c r="E45" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="21"/>
-      <c r="B46" s="18"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="6" t="s">
         <v>175</v>
       </c>
@@ -3136,8 +3693,8 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="21"/>
-      <c r="B47" s="18"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="23"/>
       <c r="C47" s="6" t="s">
         <v>176</v>
       </c>
@@ -3155,8 +3712,8 @@
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="21"/>
-      <c r="B48" s="18"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="23"/>
       <c r="C48" s="6" t="s">
         <v>177</v>
       </c>
@@ -3174,8 +3731,8 @@
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="21"/>
-      <c r="B49" s="18"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="23"/>
       <c r="C49" s="6" t="s">
         <v>184</v>
       </c>
@@ -3193,8 +3750,8 @@
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="21"/>
-      <c r="B50" s="18"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="23"/>
       <c r="C50" s="6" t="s">
         <v>185</v>
       </c>
@@ -3212,8 +3769,8 @@
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="22"/>
-      <c r="B51" s="19"/>
+      <c r="A51" s="27"/>
+      <c r="B51" s="24"/>
       <c r="C51" s="6" t="s">
         <v>186</v>
       </c>
@@ -3231,13 +3788,13 @@
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="23"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="26"/>
+      <c r="A52" s="14"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="4"/>
@@ -3485,10 +4042,10 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="23" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -3508,12 +4065,12 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="27"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="10" t="s">
+      <c r="A3" s="34"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="28" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -3527,10 +4084,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="27"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="6" t="s">
         <v>15</v>
       </c>
@@ -3542,12 +4099,12 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="27"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="10" t="s">
+      <c r="A5" s="34"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="28" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -3561,10 +4118,10 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="27"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="6" t="s">
         <v>19</v>
       </c>
@@ -3576,10 +4133,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="27"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="6" t="s">
         <v>15</v>
       </c>
@@ -3591,10 +4148,10 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="27"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="6" t="s">
         <v>25</v>
       </c>
@@ -3606,12 +4163,12 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="27"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="10" t="s">
+      <c r="A9" s="34"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="28" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -3625,10 +4182,10 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="27"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="6" t="s">
         <v>15</v>
       </c>
@@ -3640,31 +4197,31 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="27"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="14" t="s">
+      <c r="A11" s="34"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="13" t="s">
+      <c r="E11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="27"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="10" t="s">
+      <c r="A12" s="34"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="28" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="6" t="s">
@@ -3678,44 +4235,44 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="27"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="15" t="s">
+      <c r="A13" s="34"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="27"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="10" t="s">
+      <c r="A14" s="34"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="16" t="s">
+      <c r="E14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="28"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="6" t="s">
         <v>44</v>
       </c>
@@ -3727,13 +4284,13 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="4"/>
@@ -3944,29 +4501,29 @@
       <c r="A2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="31" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -3986,27 +4543,27 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="21"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="14" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="13" t="s">
+      <c r="E5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="21"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="8" t="s">
         <v>59</v>
       </c>
@@ -4024,12 +4581,12 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="21"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="10" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="28" t="s">
         <v>62</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -4038,15 +4595,15 @@
       <c r="F7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="G7" s="18" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="21"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="6" t="s">
         <v>44</v>
       </c>
@@ -4058,12 +4615,12 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="21"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="10" t="s">
+      <c r="A9" s="26"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="28" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -4077,10 +4634,10 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="21"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="6" t="s">
         <v>44</v>
       </c>
@@ -4092,12 +4649,12 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="21"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="10" t="s">
+      <c r="A11" s="26"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="28" t="s">
         <v>68</v>
       </c>
       <c r="E11" s="6" t="s">
@@ -4111,10 +4668,10 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="21"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="6" t="s">
         <v>44</v>
       </c>
@@ -4126,10 +4683,10 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="21"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="6" t="s">
         <v>73</v>
       </c>
@@ -4141,10 +4698,10 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="21"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="6" t="s">
         <v>75</v>
       </c>
@@ -4156,10 +4713,10 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="21"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="6" t="s">
         <v>76</v>
       </c>
@@ -4171,12 +4728,12 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="21"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="10" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="6" t="s">
@@ -4190,10 +4747,10 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="21"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="6" t="s">
         <v>79</v>
       </c>
@@ -4205,10 +4762,10 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="21"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
       <c r="E18" s="6" t="s">
         <v>73</v>
       </c>
@@ -4220,10 +4777,10 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="21"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="6" t="s">
         <v>75</v>
       </c>
@@ -4235,12 +4792,12 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="21"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="10" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="28" t="s">
         <v>81</v>
       </c>
       <c r="E20" s="6" t="s">
@@ -4254,14 +4811,14 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="21"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="15" t="s">
+      <c r="A21" s="26"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="12" t="s">
         <v>45</v>
       </c>
       <c r="G21" s="6" t="s">
@@ -4269,10 +4826,10 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="21"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="6" t="s">
         <v>73</v>
       </c>
@@ -4284,10 +4841,10 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="22"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
       <c r="E23" s="6" t="s">
         <v>76</v>
       </c>
@@ -4507,11 +5064,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="B4:B23"/>
     <mergeCell ref="A4:A23"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="D7:D8"/>
@@ -4520,6 +5072,11 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D11:D15"/>
     <mergeCell ref="C11:C15"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="B4:B23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -4527,264 +5084,835 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="46.28515625" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" customWidth="1"/>
+    <col min="1" max="2" width="46.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" customWidth="1"/>
+    <col min="7" max="7" width="87.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" thickBot="1">
+    <row r="1" spans="1:7" ht="19.5" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="4"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="4"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="4"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="4"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="4"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="4"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="4"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="4"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="4"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="4"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="4"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="4"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="4"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="4"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="4"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="4"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="4"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="4"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="4"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="4"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="4"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="4"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="4"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="4"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="4"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="4"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="4"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="4"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="4"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1">
+      <c r="A2" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="45"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="45"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="45"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="45"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="45"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="45"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="45"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="45"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="45"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="45"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="45"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="45"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="45"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="45"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="45"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="45"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="45"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="45"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="45"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="45"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="45"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="45"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="45"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="45"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="45"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="45"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="45"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>280</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="45"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="45"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="45"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="45"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="46"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="14"/>
+      <c r="B35" s="47"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="4"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="40" t="s">
+        <v>273</v>
+      </c>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="4"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="4"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="4"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="4"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="4"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="4"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="4"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="40" t="s">
+        <v>273</v>
+      </c>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="4"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="4"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="4"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="4"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="4"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="4"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="4"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="40" t="s">
+        <v>273</v>
+      </c>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="4"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="4"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="4"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="4"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="B2:B34"/>
+    <mergeCell ref="A2:A34"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>